<commit_message>
feat: update UI & logo company
</commit_message>
<xml_diff>
--- a/Data/Data.xlsx
+++ b/Data/Data.xlsx
@@ -221,7 +221,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="1232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="1233">
   <si>
     <t xml:space="preserve">STT</t>
   </si>
@@ -3918,6 +3918,9 @@
   </si>
   <si>
     <t xml:space="preserve">2025-08-09 10:59:48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-08-11 10:23:12</t>
   </si>
 </sst>
 </file>
@@ -7094,7 +7097,7 @@
         <v>17</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>1230</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
fix: ui & data
</commit_message>
<xml_diff>
--- a/Data/Data.xlsx
+++ b/Data/Data.xlsx
@@ -25,7 +25,7 @@
     <externalReference r:id="rId14"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1"><![CDATA['DS Final'!$A$1:$J$323]]></definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1"><![CDATA['DS Final'!$A$1:$J$324]]></definedName>
     <definedName name="_________ban1"><![CDATA['[1]Mau 02'!#REF!]]></definedName>
     <definedName name="________ban1"><![CDATA['[1]Mau 02'!#REF!]]></definedName>
     <definedName name="______ban1"><![CDATA['[1]Mau 02'!#REF!]]></definedName>
@@ -221,7 +221,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3749" uniqueCount="1225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3751" uniqueCount="1227">
   <si>
     <t xml:space="preserve">STT</t>
   </si>
@@ -3886,16 +3886,22 @@
     <t xml:space="preserve">Phó Giám đốc phụ trách Khối</t>
   </si>
   <si>
-    <t xml:space="preserve">2025-08-20 10:23:17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-08-20 10:23:26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-08-20 10:23:30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-08-20 10:24:06</t>
+    <t xml:space="preserve">2025-08-21 18:34:38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-08-21 18:45:04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-08-21 18:45:34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-08-21 18:52:51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-08-21 19:00:31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-08-21 19:02:57</t>
   </si>
 </sst>
 </file>
@@ -7115,8 +7121,8 @@
   <sheetPr/>
   <dimension ref="A1:Q324"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D1" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
@@ -7209,7 +7215,7 @@
         <v>5</v>
       </c>
       <c r="P2" s="33" t="s">
-        <v>1221</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="33" customFormat="1">
@@ -7834,6 +7840,9 @@
       <c r="L25" s="46">
         <v>7</v>
       </c>
+      <c r="P25" s="33" t="s">
+        <v>1222</v>
+      </c>
     </row>
     <row r="26" spans="1:12" s="33" customFormat="1">
       <c r="A26" s="40">
@@ -7898,6 +7907,9 @@
       <c r="L27" s="46">
         <v>19</v>
       </c>
+      <c r="P27" s="33" t="s">
+        <v>1224</v>
+      </c>
     </row>
     <row r="28" spans="1:12" s="33" customFormat="1">
       <c r="A28" s="40">
@@ -7961,6 +7973,9 @@
       </c>
       <c r="L29" s="46">
         <v>8</v>
+      </c>
+      <c r="P29" s="33" t="s">
+        <v>1223</v>
       </c>
     </row>
     <row r="30" spans="1:12" s="33" customFormat="1">
@@ -10474,7 +10489,7 @@
         <v>24</v>
       </c>
       <c r="P112" s="33" t="s">
-        <v>1222</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="113" spans="1:12" s="33" customFormat="1">
@@ -13936,9 +13951,6 @@
       <c r="L223" s="46">
         <v>10</v>
       </c>
-      <c r="P223" s="35" t="s">
-        <v>1224</v>
-      </c>
     </row>
     <row r="224" spans="1:12" s="35" customFormat="1">
       <c r="A224" s="40">
@@ -17002,66 +17014,66 @@
       <c r="L324" s="35"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J323">
+  <autoFilter ref="A1:J324">
     <extLst/>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="I202" r:id="rId1" display="vuvantien@abbank.vn"/>
-    <hyperlink ref="I206" r:id="rId2" display="vuthihuong@abbank.vn"/>
-    <hyperlink ref="I207" r:id="rId3" display="trinhhai@abbank.vn"/>
-    <hyperlink ref="I208" r:id="rId4" display="luongnd@abbank.vn"/>
-    <hyperlink ref="I209" r:id="rId5" display="nhungdt2@abbank.vn"/>
-    <hyperlink ref="I215" r:id="rId6" display="sonnam@abbank.vn"/>
-    <hyperlink ref="I216" r:id="rId7" display="trangluong@abbank.vn"/>
-    <hyperlink ref="I210" r:id="rId8" display="saulv@abbank.vn"/>
-    <hyperlink ref="I211" r:id="rId9" display="hauvv@abbank.vn"/>
-    <hyperlink ref="I212" r:id="rId10" display="tamnth@abbank.vn"/>
-    <hyperlink ref="I213" r:id="rId11" display="thaintt@abbank.vn"/>
-    <hyperlink ref="I214" r:id="rId12" display="quangnh@abbank.vn"/>
-    <hyperlink ref="I218" r:id="rId13" display="quynhvu@abbank.vn"/>
-    <hyperlink ref="I219" r:id="rId14" display="anhdiep@abbank.vn"/>
-    <hyperlink ref="I220" r:id="rId15" display="tiepkd@abbank.vn"/>
-    <hyperlink ref="I221" r:id="rId16" display="huongnguyen@abbank.vn"/>
-    <hyperlink ref="I222" r:id="rId17" display="phamhaduy@abbank.vn"/>
-    <hyperlink ref="I223" r:id="rId18" display="congpp@abbank.vn"/>
-    <hyperlink ref="I226" r:id="rId19" display="halai@abbank.vn"/>
-    <hyperlink ref="I225" r:id="rId20" display="hunglm@abbank.vn"/>
-    <hyperlink ref="I230" r:id="rId21" display="anhdn2@abbank.vn"/>
-    <hyperlink ref="I231" r:id="rId22" display="thanhnh6@abbank.vn"/>
-    <hyperlink ref="I248" r:id="rId23" display="hamtv@abbank.vn"/>
-    <hyperlink ref="I227" r:id="rId24" display="quannguyen@abbank.vn"/>
-    <hyperlink ref="I233" r:id="rId25" display="huyenntt5@abbank.vn"/>
-    <hyperlink ref="I234" r:id="rId26" display="vuongdm@abbank.vn"/>
-    <hyperlink ref="I235" r:id="rId27" display="lynguyen@abbank.vn"/>
-    <hyperlink ref="I236" r:id="rId28" display="ducnm4@abbank.vn"/>
-    <hyperlink ref="I237" r:id="rId29" display="mynh@abbank.vn"/>
-    <hyperlink ref="I239" r:id="rId30" display="nguyenphuc@abbank.vn"/>
-    <hyperlink ref="I229" r:id="rId31" display="khoanltk@abbank.vn"/>
-    <hyperlink ref="I112" r:id="rId32" display="huybq3@abbank.vn"/>
-    <hyperlink ref="I200" r:id="rId33" display="khanhho@abbank.vn"/>
-    <hyperlink ref="I217" r:id="rId34" display="hieupham@abbank.vn"/>
-    <hyperlink ref="I275" r:id="rId35" display="chiennb@abbank.vn"/>
-    <hyperlink ref="I283" r:id="rId36" display="soncn@abbank.vn"/>
-    <hyperlink ref="I284" r:id="rId37" display="sonnh@abbank.vn"/>
-    <hyperlink ref="I292" r:id="rId38" display="hant4@abbank.vn"/>
-    <hyperlink ref="I293" r:id="rId39" display="phambinhminh@abbank.vn"/>
-    <hyperlink ref="I294" r:id="rId40" display="quynhtt1@abbank.vn"/>
-    <hyperlink ref="I295" r:id="rId41" display="trangvtm@abbank.vn"/>
-    <hyperlink ref="I296" r:id="rId42" display="minhduc@abbank.vn"/>
-    <hyperlink ref="I297" r:id="rId43" display="giangpn@abbank.vn"/>
-    <hyperlink ref="I298" r:id="rId44" display="huyennt@abbank.vn"/>
-    <hyperlink ref="I299" r:id="rId45" display="vthyen@abbank.vn"/>
-    <hyperlink ref="I300" r:id="rId46" display="duongptt@abbank.vn"/>
-    <hyperlink ref="I301" r:id="rId47" display="khuongnd@abba.vn"/>
-    <hyperlink ref="I74" r:id="rId48" display="thuongdth@abbank.vn"/>
-    <hyperlink ref="I204" r:id="rId49" display="anhvct@geleximco.vn"/>
-    <hyperlink ref="I312" r:id="rId50" tooltip="mailto:hoadv@abba.vn" display="hoadv@abba.vn"/>
-    <hyperlink ref="I313" r:id="rId51" display="tuanlh3@abbank.vn"/>
-    <hyperlink ref="I4" r:id="rId52" display="tiennd2@abbank.vn"/>
-    <hyperlink ref="I314" r:id="rId53" display="luyenqd@abbank.vn"/>
-    <hyperlink ref="I317" r:id="rId54" display="kiennt@abbank.vn"/>
-    <hyperlink ref="I48" r:id="rId55" display="longpq1@abbank.vn"/>
-    <hyperlink ref="I205" r:id="rId56" display="khangdm@abbank.vn"/>
+    <hyperlink ref="I205" r:id="rId1" display="khangdm@abbank.vn"/>
+    <hyperlink ref="I202" r:id="rId2" display="vuvantien@abbank.vn"/>
+    <hyperlink ref="I206" r:id="rId3" display="vuthihuong@abbank.vn"/>
+    <hyperlink ref="I207" r:id="rId4" display="trinhhai@abbank.vn"/>
+    <hyperlink ref="I208" r:id="rId5" display="luongnd@abbank.vn"/>
+    <hyperlink ref="I209" r:id="rId6" display="nhungdt2@abbank.vn"/>
+    <hyperlink ref="I215" r:id="rId7" display="sonnam@abbank.vn"/>
+    <hyperlink ref="I216" r:id="rId8" display="trangluong@abbank.vn"/>
+    <hyperlink ref="I210" r:id="rId9" display="saulv@abbank.vn"/>
+    <hyperlink ref="I211" r:id="rId10" display="hauvv@abbank.vn"/>
+    <hyperlink ref="I212" r:id="rId11" display="tamnth@abbank.vn"/>
+    <hyperlink ref="I213" r:id="rId12" display="thaintt@abbank.vn"/>
+    <hyperlink ref="I214" r:id="rId13" display="quangnh@abbank.vn"/>
+    <hyperlink ref="I218" r:id="rId14" display="quynhvu@abbank.vn"/>
+    <hyperlink ref="I219" r:id="rId15" display="anhdiep@abbank.vn"/>
+    <hyperlink ref="I220" r:id="rId16" display="tiepkd@abbank.vn"/>
+    <hyperlink ref="I221" r:id="rId17" display="huongnguyen@abbank.vn"/>
+    <hyperlink ref="I222" r:id="rId18" display="phamhaduy@abbank.vn"/>
+    <hyperlink ref="I223" r:id="rId19" display="congpp@abbank.vn"/>
+    <hyperlink ref="I226" r:id="rId20" display="halai@abbank.vn"/>
+    <hyperlink ref="I225" r:id="rId21" display="hunglm@abbank.vn"/>
+    <hyperlink ref="I230" r:id="rId22" display="anhdn2@abbank.vn"/>
+    <hyperlink ref="I231" r:id="rId23" display="thanhnh6@abbank.vn"/>
+    <hyperlink ref="I248" r:id="rId24" display="hamtv@abbank.vn"/>
+    <hyperlink ref="I227" r:id="rId25" display="quannguyen@abbank.vn"/>
+    <hyperlink ref="I233" r:id="rId26" display="huyenntt5@abbank.vn"/>
+    <hyperlink ref="I234" r:id="rId27" display="vuongdm@abbank.vn"/>
+    <hyperlink ref="I235" r:id="rId28" display="lynguyen@abbank.vn"/>
+    <hyperlink ref="I236" r:id="rId29" display="ducnm4@abbank.vn"/>
+    <hyperlink ref="I237" r:id="rId30" display="mynh@abbank.vn"/>
+    <hyperlink ref="I239" r:id="rId31" display="nguyenphuc@abbank.vn"/>
+    <hyperlink ref="I229" r:id="rId32" display="khoanltk@abbank.vn"/>
+    <hyperlink ref="I112" r:id="rId33" display="huybq3@abbank.vn"/>
+    <hyperlink ref="I200" r:id="rId34" display="khanhho@abbank.vn"/>
+    <hyperlink ref="I217" r:id="rId35" display="hieupham@abbank.vn"/>
+    <hyperlink ref="I275" r:id="rId36" display="chiennb@abbank.vn"/>
+    <hyperlink ref="I283" r:id="rId37" display="soncn@abbank.vn"/>
+    <hyperlink ref="I284" r:id="rId38" display="sonnh@abbank.vn"/>
+    <hyperlink ref="I292" r:id="rId39" display="hant4@abbank.vn"/>
+    <hyperlink ref="I293" r:id="rId40" display="phambinhminh@abbank.vn"/>
+    <hyperlink ref="I294" r:id="rId41" display="quynhtt1@abbank.vn"/>
+    <hyperlink ref="I295" r:id="rId42" display="trangvtm@abbank.vn"/>
+    <hyperlink ref="I296" r:id="rId43" display="minhduc@abbank.vn"/>
+    <hyperlink ref="I297" r:id="rId44" display="giangpn@abbank.vn"/>
+    <hyperlink ref="I298" r:id="rId45" display="huyennt@abbank.vn"/>
+    <hyperlink ref="I299" r:id="rId46" display="vthyen@abbank.vn"/>
+    <hyperlink ref="I300" r:id="rId47" display="duongptt@abbank.vn"/>
+    <hyperlink ref="I301" r:id="rId48" display="khuongnd@abba.vn"/>
+    <hyperlink ref="I74" r:id="rId49" display="thuongdth@abbank.vn"/>
+    <hyperlink ref="I204" r:id="rId50" display="anhvct@geleximco.vn"/>
+    <hyperlink ref="I312" r:id="rId51" tooltip="mailto:hoadv@abba.vn" display="hoadv@abba.vn"/>
+    <hyperlink ref="I313" r:id="rId52" display="tuanlh3@abbank.vn"/>
+    <hyperlink ref="I4" r:id="rId53" display="tiennd2@abbank.vn"/>
+    <hyperlink ref="I314" r:id="rId54" display="luyenqd@abbank.vn"/>
+    <hyperlink ref="I317" r:id="rId55" display="kiennt@abbank.vn"/>
+    <hyperlink ref="I48" r:id="rId56" display="longpq1@abbank.vn"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="12" fitToWidth="0" fitToHeight="0" orientation="landscape"/>

</xml_diff>